<commit_message>
power board and midplate updates (mostly finalized)
</commit_message>
<xml_diff>
--- a/MidPlate/Midplate BOM Jan 15.xlsx
+++ b/MidPlate/Midplate BOM Jan 15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The Bots\Electrical\MidPlate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E6EB3A-1071-4851-8603-78EBD13E8D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5D6854-29F2-4268-A31A-C6C1CDA2A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5112" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Midplate BOM Jan 14" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
   <si>
     <t>Ref</t>
   </si>
@@ -257,9 +257,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Board Cost</t>
-  </si>
-  <si>
     <t>C440198</t>
   </si>
   <si>
@@ -330,6 +327,54 @@
   </si>
   <si>
     <t>usd to cad</t>
+  </si>
+  <si>
+    <t>3-794636-6</t>
+  </si>
+  <si>
+    <t>0297015.WXT</t>
+  </si>
+  <si>
+    <t>FIT0582</t>
+  </si>
+  <si>
+    <t>BM04B-GHS-TBT</t>
+  </si>
+  <si>
+    <t>2-1445053-2</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Bottom side components and extra stuff</t>
+  </si>
+  <si>
+    <t>R4, R5</t>
+  </si>
+  <si>
+    <t>J4, J5</t>
+  </si>
+  <si>
+    <t>RMCF0603FT110R</t>
+  </si>
+  <si>
+    <t>Digikey cost</t>
+  </si>
+  <si>
+    <t>JLC cost</t>
+  </si>
+  <si>
+    <t>extra digikey</t>
   </si>
 </sst>
 </file>
@@ -1185,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1224,7 +1269,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -1328,7 +1373,7 @@
         <v>JLC</v>
       </c>
       <c r="T3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -1339,10 +1384,10 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4">
         <v>0.317</v>
@@ -1377,7 +1422,7 @@
         <v>JLC</v>
       </c>
       <c r="P4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q4" s="3">
         <v>33.590000000000003</v>
@@ -1398,7 +1443,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1">
         <v>0.05</v>
@@ -1433,13 +1478,13 @@
         <v>JLC</v>
       </c>
       <c r="P5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q5" s="3">
         <v>10.78</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -1488,13 +1533,13 @@
         <v>JLC</v>
       </c>
       <c r="P6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q6" s="3">
         <v>2.02</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -1543,7 +1588,7 @@
         <v>JLC</v>
       </c>
       <c r="P7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q7" s="3">
         <v>62.46</v>
@@ -1553,10 +1598,10 @@
         <v>93.41</v>
       </c>
       <c r="S7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -1605,13 +1650,13 @@
         <v>JLC</v>
       </c>
       <c r="P8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="3">
         <v>30.95</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -1631,12 +1676,12 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>H9*8</f>
+        <v>8</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>16.8</v>
+        <v>13.44</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="2"/>
@@ -1644,20 +1689,20 @@
       </c>
       <c r="L9">
         <f t="shared" si="3"/>
-        <v>16.8</v>
+        <v>13.44</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="4"/>
         <v>DIGIKEY</v>
       </c>
       <c r="P9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q9" s="3">
         <v>1.85</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -1671,7 +1716,7 @@
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10">
         <v>0.49519999999999997</v>
@@ -1706,13 +1751,13 @@
         <v>JLC</v>
       </c>
       <c r="P10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q10" s="3">
         <v>0.57999999999999996</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -1726,7 +1771,7 @@
         <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11">
         <v>0.60599999999999998</v>
@@ -1774,7 +1819,7 @@
         <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12">
         <v>0.26900000000000002</v>
@@ -1789,27 +1834,27 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>H12*8</f>
+        <v>8</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>2.6900000000000004</v>
+        <v>2.1520000000000001</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>4.4350000000000005</v>
+        <v>4.3559999999999999</v>
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
-        <v>2.6900000000000004</v>
+        <v>2.1520000000000001</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="4"/>
         <v>DIGIKEY</v>
       </c>
       <c r="P12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q12" s="3">
         <v>74.34</v>
@@ -1844,27 +1889,27 @@
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>H13*8</f>
+        <v>8</v>
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>0.42000000000000004</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>4.2050000000000001</v>
+        <v>4.1719999999999997</v>
       </c>
       <c r="L13">
         <f t="shared" si="3"/>
-        <v>0.42000000000000004</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="4"/>
         <v>DIGIKEY</v>
       </c>
       <c r="P13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q13" s="3">
         <f>SUM(Q4:Q12)</f>
@@ -1921,7 +1966,7 @@
         <v>JLC</v>
       </c>
       <c r="P14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q14" s="3">
         <f>0.12*Q13</f>
@@ -1978,7 +2023,7 @@
         <v>JLC</v>
       </c>
       <c r="P15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q15" s="3">
         <v>17.5</v>
@@ -2137,11 +2182,11 @@
       </c>
       <c r="Q18" s="3">
         <f>Q16+N22</f>
-        <v>293.74840000000006</v>
+        <v>372.69568000000004</v>
       </c>
       <c r="T18" s="3">
         <f>T16+J22</f>
-        <v>313.38469999999995</v>
+        <v>306.73869999999999</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
@@ -2161,12 +2206,12 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>H19*8</f>
+        <v>8</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>13.32</v>
+        <v>10.656000000000001</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="2"/>
@@ -2174,22 +2219,22 @@
       </c>
       <c r="L19">
         <f t="shared" si="3"/>
-        <v>13.32</v>
+        <v>10.656000000000001</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="4"/>
         <v>DIGIKEY</v>
       </c>
       <c r="P19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q19" s="3">
         <f>Q18/10</f>
-        <v>29.374840000000006</v>
+        <v>37.269568000000007</v>
       </c>
       <c r="T19" s="3">
         <f>T18/10</f>
-        <v>31.338469999999994</v>
+        <v>30.673870000000001</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
@@ -2247,38 +2292,38 @@
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="J22">
         <f>SUM(J2:J20)</f>
-        <v>221.43439999999998</v>
+        <v>214.78839999999997</v>
       </c>
       <c r="K22" t="s">
         <v>73</v>
       </c>
       <c r="L22">
         <f>SUM(L2:L20)</f>
-        <v>128.49380000000002</v>
+        <v>121.84780000000001</v>
       </c>
       <c r="M22" s="2">
         <f>SUMIF(M2:M20,"JLC",L2:L20)</f>
         <v>94.803799999999995</v>
       </c>
       <c r="N22">
-        <f>L22-M22</f>
-        <v>33.690000000000026</v>
+        <f>(L22-M22+J41)*1.12</f>
+        <v>112.63728000000003</v>
       </c>
       <c r="Q22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="K23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L23">
-        <v>33.590000000000003</v>
+      <c r="M23" t="s">
+        <v>112</v>
+      </c>
+      <c r="N23" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24">
         <v>1.3497425000000001</v>
@@ -2290,6 +2335,200 @@
         <v>3.8687499999999999</v>
       </c>
     </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>3568</v>
+      </c>
+      <c r="E28">
+        <v>1.68</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28">
+        <f>E28*I28</f>
+        <v>13.44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>15</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ref="J29:J40" si="5">E29*I29</f>
+        <v>6.1349999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31">
+        <v>8.85</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="5"/>
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36">
+        <v>1.88</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="5"/>
+        <v>15.04</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37">
+        <v>3.7</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>8</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="5"/>
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39">
+        <v>2.3E-2</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>10</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="5"/>
+        <v>0.22999999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40">
+        <v>2.3E-2</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="5"/>
+        <v>0.22999999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>113</v>
+      </c>
+      <c r="J41">
+        <f>SUM(J28:J40)</f>
+        <v>73.525000000000006</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
midplate - with alt parts
</commit_message>
<xml_diff>
--- a/MidPlate/Midplate BOM Jan 15.xlsx
+++ b/MidPlate/Midplate BOM Jan 15.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henry\Documents\Documents\University\GitHub\The_Bots\Electrical\MidPlate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8BC7A1-AF8F-4E48-9413-0CD36D896BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AA5FEA-F346-4885-AA7D-CC3AE64D0230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5112" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Midplate BOM Jan 14" sheetId="1" r:id="rId1"/>
@@ -1275,7 +1275,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>